<commit_message>
Added tests concerning adding track to user's playlist by other user
</commit_message>
<xml_diff>
--- a/src/test/java/docs/SpotifyAPITestReport.xlsx
+++ b/src/test/java/docs/SpotifyAPITestReport.xlsx
@@ -5,13 +5,15 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="CP_Create Playlist" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="ATTP_Add Track To Playlist" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
+    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">'ATTP_Add Track To Playlist'!$A$1:$C$35</definedName>
     <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">'CP_Create Playlist'!$A$1:$F$21</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="132">
   <si>
     <t xml:space="preserve">Test Report from Spotify API Tests</t>
   </si>
@@ -42,6 +44,9 @@
   </si>
   <si>
     <t xml:space="preserve">Create Playlist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add Track To Playlist</t>
   </si>
   <si>
     <t xml:space="preserve">Test case id</t>
@@ -209,6 +214,217 @@
   </si>
   <si>
     <t xml:space="preserve">Don’t create playlist with invalid token</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ATTP1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add single track to empty playlist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ATTP2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add single track to empty playlist at position 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ATTP3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Don't add track to empty playlist at position other then 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ATTP4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add single track to populated playlist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ATTP5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add single track to the beginning of populated playlist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ATTP6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add single track to populated playlist at position lower than limit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ATTP7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add single track to populated playlist at position greater or equal to limit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ATTP8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Don’t add track at position higher than playlist size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ATTP9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add tracks separately to empty playlist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ATTP10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add the same track twice in separated request to empty playlist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ATTP11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add tracks in one request to empty playlist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ATTP12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add the same track twice in one request to empty playlist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ATTP13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add the same track twice in one request to populated playlist at given position</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ATTP14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Don't add more than 100 tracks in one request to playlist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ATTP15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add tracks to populated playlist at current page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ATTP16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add tracks to populated playlist partially shifted to next page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ATTP17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add tracks to populated playlist at next page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ATTP18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add max number of tracks per request to populated playlist at given position</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ATTP19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add tracks to the beginning of playlist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ATTP20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shift tracks in current page when tracks added to playlist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ATTP21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shift tracks partially from current to next page when tracks added to playlist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ATTP22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shift tracks only in second page when tracks added to playlist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ATTP23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Don’t add tracks at invalid position</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ATTP24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Don’t add tracks at negative position</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ATTP25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Don't add track if no uri param provided</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ATTP26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Don't add track if invalid uri provided</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ATTP27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Don't add track if non existing uri provided</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ATTP28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Don't add track if empty playlist id param provided</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ATTP29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Don't add track if invalid playlist id provided</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ATTP30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Don't add track if empty token provided</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ATTP31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Don't add track if invalid token provided</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ATTP32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Don't add other items different than tracks to playlist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ATTP33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Don't add items to other user's non collaborative playlist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ATTP34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add items to other user's private collaborative playlist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Status code should be 201.
+Other user should be able to add a track to private collaborative playlist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Status code is 403. Message in response is “You cannot add tracks to a playlist you don't own.”</t>
   </si>
 </sst>
 </file>
@@ -219,7 +435,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yy"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -243,6 +459,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -296,7 +519,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -322,6 +545,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -401,21 +632,25 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:B7"/>
+  <dimension ref="A2:B9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.15"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -436,15 +671,23 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="n">
-        <v>44854</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+        <v>44784</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="2"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B8" s="0" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -465,13 +708,13 @@
   </sheetPr>
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
+      <selection pane="bottomLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.3"/>
@@ -481,295 +724,295 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
     </row>
     <row r="3" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
     </row>
     <row r="4" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
     </row>
     <row r="5" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
     </row>
     <row r="6" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
     </row>
     <row r="8" customFormat="false" ht="58.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
     </row>
     <row r="10" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
     </row>
     <row r="11" customFormat="false" ht="69.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
     </row>
     <row r="13" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
     </row>
     <row r="15" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
     </row>
     <row r="16" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
     </row>
     <row r="17" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
     </row>
     <row r="18" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
     </row>
     <row r="19" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
     </row>
     <row r="20" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
     </row>
     <row r="21" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
@@ -785,4 +1028,436 @@
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F35"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="5" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="5" width="50.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="41.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.07"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:C35"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>